<commit_message>
added the To Try places to the map, color legend, and wrote code in case I want to use custom markers at some point. Note: buford hwy locations removed NE to actually map
</commit_message>
<xml_diff>
--- a/ATL-Food-and-Drink-Review-List.xlsx
+++ b/ATL-Food-and-Drink-Review-List.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="411">
   <si>
     <t>The designations of "Vegan" are used to roughly quantify the percentage of the menu items that are vegan:</t>
   </si>
@@ -53,141 +53,273 @@
     <t>Type</t>
   </si>
   <si>
+    <t>Location</t>
+  </si>
+  <si>
     <t>Vegan Wangs</t>
   </si>
   <si>
-    <t>Restaurant</t>
+    <t>Restaurants</t>
+  </si>
+  <si>
+    <t>833 Cascade Rd Suite A, Atlanta, GA 30310</t>
   </si>
   <si>
     <t xml:space="preserve">Slutty Vegan </t>
   </si>
   <si>
-    <t>Bahel Ethipoian</t>
+    <t>1542 Ralph David Abernathy Blvd SW, Atlanta, GA 30310</t>
+  </si>
+  <si>
+    <t>Bahel Ethipoian Restaurant</t>
+  </si>
+  <si>
+    <t>3125 Briarcliff Rd NE ste c, Atlanta, GA 30329</t>
   </si>
   <si>
     <t>Maepole</t>
   </si>
   <si>
+    <t>72 Georgia Ave SE Unit 500, Atlanta, GA 30312</t>
+  </si>
+  <si>
     <t>Pom Court @ Hotel Granada</t>
   </si>
   <si>
+    <t>1302 W Peachtree St NW, Atlanta, GA 30309</t>
+  </si>
+  <si>
     <t>HC Biergarten</t>
   </si>
   <si>
     <t>Bars</t>
   </si>
   <si>
+    <t>640 Reed St SE, Atlanta, GA 30312</t>
+  </si>
+  <si>
     <t>Sweet Water Brewing</t>
   </si>
   <si>
+    <t>195 Ottley Drive Northeast, Atlanta, GA 30324</t>
+  </si>
+  <si>
     <t>Three Taverns Imaginarium</t>
   </si>
   <si>
-    <t>The Rooftop at Clarmont</t>
+    <t>777 Memorial Dr SE Suite B103, Atlanta, GA 30316</t>
+  </si>
+  <si>
+    <t>The Rooftop at Clermont</t>
+  </si>
+  <si>
+    <t>789 Ponce De Leon Ave NE, Atlanta, GA 30306</t>
   </si>
   <si>
     <t>Ranger Station Speakeasy</t>
   </si>
   <si>
+    <t>684 John Wesley Dobbs Ave NE Unit J, Atlanta, GA 30312</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tabla </t>
   </si>
   <si>
+    <t>77 12th St NE #2, Atlanta, GA 30309</t>
+  </si>
+  <si>
     <t>Yakitori Kona</t>
   </si>
   <si>
+    <t>1004 Virginia Ave NE, Atlanta, GA 30306</t>
+  </si>
+  <si>
     <t>Vegan Food Social (ATL utility works)</t>
   </si>
   <si>
+    <t>2903 RN Martin St, East Point, GA 30344</t>
+  </si>
+  <si>
     <t>Cafe Sunflower</t>
   </si>
   <si>
+    <t>2140 Peachtree Rd, Atlanta, GA 30309</t>
+  </si>
+  <si>
     <t>Coyote's Mexican Grill</t>
   </si>
   <si>
+    <t>105 Sycamore Pl, Decatur, GA 30030</t>
+  </si>
+  <si>
     <t>Arepa Mia</t>
   </si>
   <si>
+    <t>10 N Clarendon Ave suite a, Avondale Estates, GA 30002</t>
+  </si>
+  <si>
     <t>Chai Pani</t>
   </si>
   <si>
-    <t>Metrpolis Cafe</t>
-  </si>
-  <si>
-    <t>Ruby Chows</t>
+    <t>406 W Ponce de Leon Ave, Decatur, GA 30030</t>
+  </si>
+  <si>
+    <t>Ruby Chow</t>
+  </si>
+  <si>
+    <t>620 Glen Iris Dr NE Unit C-1, Atlanta, GA 30308</t>
   </si>
   <si>
     <t>Masterpiece</t>
   </si>
   <si>
-    <t>Whoopsies (can be vegan)</t>
-  </si>
-  <si>
-    <t>Estrellita Filipino (cant be vegan)</t>
-  </si>
-  <si>
-    <t>Bacelona Tapas</t>
+    <t>3940 Buford Hwy, Duluth, GA 30096</t>
+  </si>
+  <si>
+    <t>Whoopsies</t>
+  </si>
+  <si>
+    <t>1 Moreland Ave SE suite c, Atlanta, GA 30316</t>
+  </si>
+  <si>
+    <t>Estrellita Filipino</t>
+  </si>
+  <si>
+    <t>580 Woodward Ave SE, Atlanta, GA 30312</t>
+  </si>
+  <si>
+    <t>Bacelona Wine Bar</t>
+  </si>
+  <si>
+    <t>240 North Highland Avenue Northeast, Atlanta, GA 30307</t>
   </si>
   <si>
     <t>Pho Bac</t>
   </si>
   <si>
-    <t>Kamayan</t>
-  </si>
-  <si>
-    <t>Vegreen</t>
-  </si>
-  <si>
-    <t>Lees Bakery</t>
-  </si>
-  <si>
-    <t>Chat Patti</t>
-  </si>
-  <si>
-    <t>Desi Spice</t>
+    <t>4897 Buford Hwy suite 106, Chamblee, GA 30341</t>
+  </si>
+  <si>
+    <t>Kamayan ATL - Filipino Restaurant</t>
+  </si>
+  <si>
+    <t>5150 Buford Hwy A230, Doraville, GA 30340</t>
+  </si>
+  <si>
+    <t>VeGreen Vegan Fusion Restaurant</t>
+  </si>
+  <si>
+    <t>3780 Old Norcross Rd #106, Duluth, GA 30096</t>
+  </si>
+  <si>
+    <t>Lee's Bakery</t>
+  </si>
+  <si>
+    <t>4005 Buford Hwy Suite C, Atlanta, GA 30345</t>
+  </si>
+  <si>
+    <t>Chat Patti Indian Vegetarian Restaurant</t>
+  </si>
+  <si>
+    <t>1707 Church St, Decatur, GA 30033</t>
+  </si>
+  <si>
+    <t>Desi Spice Indian Cuisine</t>
+  </si>
+  <si>
+    <t>Promenade, 931 Monroe Dr NE, Atlanta, GA 30308</t>
   </si>
   <si>
     <t>Bakaris Pizza</t>
   </si>
   <si>
+    <t>576 Lee St SW, Atlanta, GA 30310</t>
+  </si>
+  <si>
     <t>Shoya Izakaya</t>
   </si>
   <si>
+    <t>6035 Peachtree Rd A101, Doraville, GA 30340</t>
+  </si>
+  <si>
     <t>My Parents Basement</t>
   </si>
   <si>
+    <t>22 N Avondale Rd, Avondale Estates, GA 30002</t>
+  </si>
+  <si>
     <t>Moonlight</t>
   </si>
   <si>
-    <t>Stereo ATL</t>
-  </si>
-  <si>
-    <t>Jikssa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Restaurant </t>
-  </si>
-  <si>
-    <t>Dekalb Famers Market</t>
+    <t>800 Rankin St NE, Atlanta, GA 30308</t>
+  </si>
+  <si>
+    <t>Stereo</t>
+  </si>
+  <si>
+    <t>900 DeKalb Ave NE suite f, Atlanta, GA 30307</t>
+  </si>
+  <si>
+    <t>Your DeKalb Farmers Market</t>
   </si>
   <si>
     <t xml:space="preserve">Grocery store </t>
   </si>
   <si>
+    <t>3000 E Ponce de Leon Ave, Decatur, GA 30030</t>
+  </si>
+  <si>
     <t>TESO Life</t>
   </si>
   <si>
     <t>Grocery store</t>
   </si>
   <si>
+    <t>2180 Pleasant Hill Rd SUITE F, Duluth, GA 30096</t>
+  </si>
+  <si>
     <t>Lov'n it live</t>
   </si>
   <si>
+    <t>2796 E Point St, East Point, GA 30344</t>
+  </si>
+  <si>
     <t>Planted soul</t>
   </si>
   <si>
+    <t>3569 Main St, College Park, GA 30337</t>
+  </si>
+  <si>
     <t>Yalda</t>
   </si>
   <si>
+    <t>980 Howell Mill Rd Suite 4, Atlanta, GA 30318</t>
+  </si>
+  <si>
+    <t>Madre Selva</t>
+  </si>
+  <si>
+    <t>570 Main St NE, Atlanta, GA 30324</t>
+  </si>
+  <si>
+    <t>Okiboru Tsukemen &amp; Ramen</t>
+  </si>
+  <si>
+    <t>2277 Peachtree Rd NE B, Atlanta, GA 30309</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mellow Mushroom </t>
+  </si>
+  <si>
+    <t>931 Monroe Dr NE, Atlanta, GA 30308</t>
+  </si>
+  <si>
+    <t>La Hacienda Midtown</t>
+  </si>
+  <si>
+    <t>900 Monroe Dr NE, Atlanta, GA 30308</t>
+  </si>
+  <si>
     <t>Cuisine</t>
   </si>
   <si>
@@ -203,9 +335,6 @@
     <t>Additional Notes</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
     <t>Delbar (Inman Park)</t>
   </si>
   <si>
@@ -215,7 +344,7 @@
     <t>Partially</t>
   </si>
   <si>
-    <t>870 Inman Vlg Pkwy NE Suite 1, Atlanta, GA 30307</t>
+    <t>870 Inman Villge Pkwy NE Suite 1, Atlanta, GA 30307</t>
   </si>
   <si>
     <t>Little Bear</t>
@@ -305,7 +434,7 @@
     <t>$4-5 for a Bahn Mi. Super cheap. Best Bahn Mi i've had (Joe) in a long time.</t>
   </si>
   <si>
-    <t>5150 Buford Hwy NE, Doraville, GA 30340</t>
+    <t>5150 Buford Hwy, Doraville, GA 30340</t>
   </si>
   <si>
     <t>Desta</t>
@@ -329,7 +458,7 @@
     <t>good soup dumpling and eggplant</t>
   </si>
   <si>
-    <t>5141 Buford Hwy NE Suite C, Doraville, GA 30340</t>
+    <t>5141 Buford Hwy Suite C, Doraville, GA 30340</t>
   </si>
   <si>
     <t>Vegan House of Pancakes</t>
@@ -407,9 +536,6 @@
     <t>vibes were high, French fries and mussels were a good value</t>
   </si>
   <si>
-    <t>800 Rankin St NE, Atlanta, GA 30308</t>
-  </si>
-  <si>
     <t>Argosy</t>
   </si>
   <si>
@@ -461,7 +587,7 @@
     <t>solid vegan street tacos</t>
   </si>
   <si>
-    <t>3795 Presidential Pkwy Suite FP-10, Atlanta, GA 30340</t>
+    <t>3795 Presidential Pkwy, Atlanta, GA 30340</t>
   </si>
   <si>
     <t>El Tesoro</t>
@@ -494,7 +620,7 @@
     <t>massive menu of eats, curry laksa is the move</t>
   </si>
   <si>
-    <t>5000 Buford Hwy NE, Chamblee, GA 30341</t>
+    <t>5000 Buford Hwy, Chamblee, GA 30341</t>
   </si>
   <si>
     <t>Kitty Dare</t>
@@ -539,7 +665,7 @@
     <t>tasty Vietnamese but tofu dish barely had any tofu, Pho is supposed to be the best in ATL but didn't have</t>
   </si>
   <si>
-    <t>4051 Buford Hwy NE, Atlanta, GA 30345</t>
+    <t>4051 Buford Hwy, Atlanta, GA 30345</t>
   </si>
   <si>
     <t>Harmony Vegetarian</t>
@@ -548,7 +674,7 @@
     <t>good Chinese vegetarian spot with more vegan options and better prices than other options on the list (e.g. Northern China eatery)</t>
   </si>
   <si>
-    <t>Orient Center Shopping Plaza, 4897 Buford Hwy NE #109, Chamblee, GA 30341</t>
+    <t>Orient Center Shopping Plaza, 4897 Buford Hwy #109, Chamblee, GA 30341</t>
   </si>
   <si>
     <t>Woody’s Cheesesteaks</t>
@@ -971,9 +1097,6 @@
     <t>the bar outside the steakhouse</t>
   </si>
   <si>
-    <t>800 Rankin St NE 1st Floor, Atlanta, GA 30308</t>
-  </si>
-  <si>
     <t>Finca to Filter O4W</t>
   </si>
   <si>
@@ -1010,16 +1133,13 @@
     <t>only had nutella bun, but good</t>
   </si>
   <si>
-    <t>5150 Buford Hwy NE A-100, Doraville, GA 30340</t>
-  </si>
-  <si>
     <t>Cafe Maiko</t>
   </si>
   <si>
     <t>Match Tea</t>
   </si>
   <si>
-    <t>Partiall</t>
+    <t>5306 Buford Hwy, Atlanta, GA 30340</t>
   </si>
   <si>
     <t>Monday Night Brewing - The Garage</t>
@@ -1037,9 +1157,6 @@
     <t>good vibes, great frozen lemonade</t>
   </si>
   <si>
-    <t>684 John Wesley Dobbs Ave NE Unit J, Atlanta, GA 30312</t>
-  </si>
-  <si>
     <t>Strangers in Paradise</t>
   </si>
   <si>
@@ -1136,7 +1253,7 @@
     <t>Bold Monk Brewing Co.</t>
   </si>
   <si>
-    <t>1737 Ellsworth Industrial Blvd NW suite d-1, Atlanta, GA 30318</t>
+    <t>1737 Ellsworth Industrial Blvd NW, Atlanta, GA 30318</t>
   </si>
 </sst>
 </file>
@@ -1497,322 +1614,470 @@
       <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>17</v>
+        <v>80</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>47</v>
+        <v>83</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>49</v>
+        <v>12</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>51</v>
+        <v>12</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>47</v>
+        <v>12</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>47</v>
+        <v>12</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>47</v>
+        <v>12</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1839,22 +2104,22 @@
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>56</v>
+        <v>100</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -1877,13 +2142,13 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D2" s="5">
         <v>4.5</v>
@@ -1894,7 +2159,7 @@
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="5" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -1917,13 +2182,13 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D3" s="5">
         <v>4.5</v>
@@ -1933,10 +2198,10 @@
         <v>9</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -1959,13 +2224,13 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>70</v>
+        <v>113</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="D4" s="5">
         <v>4.5</v>
@@ -1975,10 +2240,10 @@
         <v>9</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>72</v>
+        <v>115</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>73</v>
+        <v>116</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -2001,13 +2266,13 @@
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D5" s="5">
         <v>4.5</v>
@@ -2017,10 +2282,10 @@
         <v>9</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>78</v>
+        <v>121</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -2043,13 +2308,13 @@
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>80</v>
+        <v>123</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="D6" s="5">
         <v>4.0</v>
@@ -2060,7 +2325,7 @@
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="5" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -2083,13 +2348,13 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>83</v>
+        <v>126</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>84</v>
+        <v>127</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D7" s="5">
         <v>4.0</v>
@@ -2099,10 +2364,10 @@
         <v>8</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>85</v>
+        <v>128</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -2125,13 +2390,13 @@
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>87</v>
+        <v>130</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>88</v>
+        <v>131</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D8" s="5">
         <v>4.0</v>
@@ -2141,10 +2406,10 @@
         <v>8</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>89</v>
+        <v>132</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>90</v>
+        <v>133</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -2167,13 +2432,13 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>91</v>
+        <v>134</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>92</v>
+        <v>135</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D9" s="5">
         <v>4.0</v>
@@ -2183,10 +2448,10 @@
         <v>8</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>93</v>
+        <v>136</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>94</v>
+        <v>137</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -2209,13 +2474,13 @@
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>96</v>
+        <v>139</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D10" s="5">
         <v>4.0</v>
@@ -2225,10 +2490,10 @@
         <v>8</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>97</v>
+        <v>140</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -2251,13 +2516,13 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>99</v>
+        <v>142</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D11" s="5">
         <v>3.75</v>
@@ -2267,10 +2532,10 @@
         <v>7.5</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>102</v>
+        <v>145</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -2293,13 +2558,13 @@
     </row>
     <row r="12">
       <c r="A12" s="5" t="s">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>104</v>
+        <v>147</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="D12" s="5">
         <v>3.75</v>
@@ -2309,10 +2574,10 @@
         <v>7.5</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>105</v>
+        <v>148</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -2335,13 +2600,13 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>107</v>
+        <v>150</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D13" s="5">
         <v>3.75</v>
@@ -2351,10 +2616,10 @@
         <v>7.5</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>109</v>
+        <v>152</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>110</v>
+        <v>153</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -2377,13 +2642,13 @@
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>111</v>
+        <v>154</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>112</v>
+        <v>155</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D14" s="5">
         <v>3.75</v>
@@ -2393,10 +2658,10 @@
         <v>7.5</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>113</v>
+        <v>156</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>114</v>
+        <v>157</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -2419,13 +2684,13 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>115</v>
+        <v>158</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>116</v>
+        <v>159</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="D15" s="5">
         <v>3.5</v>
@@ -2435,10 +2700,10 @@
         <v>7</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>117</v>
+        <v>160</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>118</v>
+        <v>161</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
@@ -2461,13 +2726,13 @@
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>119</v>
+        <v>162</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>120</v>
+        <v>163</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>121</v>
+        <v>164</v>
       </c>
       <c r="D16" s="5">
         <v>3.5</v>
@@ -2478,7 +2743,7 @@
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="5" t="s">
-        <v>122</v>
+        <v>165</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
@@ -2501,13 +2766,13 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>123</v>
+        <v>166</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>116</v>
+        <v>159</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D17" s="5">
         <v>3.5</v>
@@ -2517,10 +2782,10 @@
         <v>7</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>124</v>
+        <v>167</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -2543,13 +2808,13 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>125</v>
+        <v>168</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>126</v>
+        <v>169</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D18" s="5">
         <v>3.5</v>
@@ -2559,10 +2824,10 @@
         <v>7</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>127</v>
+        <v>170</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>128</v>
+        <v>76</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
@@ -2585,13 +2850,13 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>129</v>
+        <v>171</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>130</v>
+        <v>172</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D19" s="5">
         <v>3.5</v>
@@ -2601,10 +2866,10 @@
         <v>7</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>131</v>
+        <v>173</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>132</v>
+        <v>174</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
@@ -2627,13 +2892,13 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>133</v>
+        <v>175</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>134</v>
+        <v>176</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>135</v>
+        <v>177</v>
       </c>
       <c r="D20" s="5">
         <v>3.5</v>
@@ -2643,10 +2908,10 @@
         <v>7</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>136</v>
+        <v>178</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>137</v>
+        <v>179</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
@@ -2669,13 +2934,13 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>138</v>
+        <v>180</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>126</v>
+        <v>169</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D21" s="5">
         <v>3.5</v>
@@ -2685,10 +2950,10 @@
         <v>7</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>139</v>
+        <v>181</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>140</v>
+        <v>182</v>
       </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
@@ -2711,13 +2976,13 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>141</v>
+        <v>183</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>142</v>
+        <v>184</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D22" s="5">
         <v>3.5</v>
@@ -2728,7 +2993,7 @@
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="1" t="s">
-        <v>143</v>
+        <v>185</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -2751,13 +3016,13 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="D23" s="5">
         <v>3.5</v>
@@ -2767,10 +3032,10 @@
         <v>7</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>145</v>
+        <v>187</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>146</v>
+        <v>188</v>
       </c>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -2793,13 +3058,13 @@
     </row>
     <row r="24">
       <c r="A24" s="5" t="s">
-        <v>147</v>
+        <v>189</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D24" s="5">
         <v>3.5</v>
@@ -2809,10 +3074,10 @@
         <v>7</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>148</v>
+        <v>190</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>149</v>
+        <v>191</v>
       </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -2835,13 +3100,13 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="s">
-        <v>150</v>
+        <v>192</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>151</v>
+        <v>193</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D25" s="5">
         <v>3.5</v>
@@ -2851,10 +3116,10 @@
         <v>7</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>152</v>
+        <v>194</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>153</v>
+        <v>195</v>
       </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
@@ -2877,13 +3142,13 @@
     </row>
     <row r="26">
       <c r="A26" s="5" t="s">
-        <v>154</v>
+        <v>196</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>155</v>
+        <v>197</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D26" s="5">
         <v>3.5</v>
@@ -2893,10 +3158,10 @@
         <v>7</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>156</v>
+        <v>198</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>157</v>
+        <v>199</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -2919,13 +3184,13 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="s">
-        <v>158</v>
+        <v>200</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>159</v>
+        <v>201</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D27" s="5">
         <v>3.5</v>
@@ -2935,10 +3200,10 @@
         <v>7</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>160</v>
+        <v>202</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>161</v>
+        <v>203</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -2961,13 +3226,13 @@
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>162</v>
+        <v>204</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>163</v>
+        <v>205</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="D28" s="5">
         <v>3.5</v>
@@ -2977,10 +3242,10 @@
         <v>7</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>165</v>
+        <v>207</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -3003,13 +3268,13 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>166</v>
+        <v>208</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>167</v>
+        <v>209</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D29" s="5">
         <v>3.5</v>
@@ -3019,10 +3284,10 @@
         <v>7</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>168</v>
+        <v>210</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>169</v>
+        <v>211</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -3045,13 +3310,13 @@
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>170</v>
+        <v>212</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>92</v>
+        <v>135</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D30" s="5">
         <v>3.5</v>
@@ -3061,10 +3326,10 @@
         <v>7</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>171</v>
+        <v>213</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>172</v>
+        <v>214</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
@@ -3087,13 +3352,13 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>173</v>
+        <v>215</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>100</v>
+        <v>143</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>121</v>
+        <v>164</v>
       </c>
       <c r="D31" s="5">
         <v>3.5</v>
@@ -3103,10 +3368,10 @@
         <v>7</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>174</v>
+        <v>216</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>175</v>
+        <v>217</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
@@ -3129,13 +3394,13 @@
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>176</v>
+        <v>218</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>177</v>
+        <v>219</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>178</v>
+        <v>220</v>
       </c>
       <c r="D32" s="5">
         <v>3.5</v>
@@ -3145,10 +3410,10 @@
         <v>7</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>179</v>
+        <v>221</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>180</v>
+        <v>222</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
@@ -3171,13 +3436,13 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>181</v>
+        <v>223</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="D33" s="1">
         <v>3.5</v>
@@ -3187,10 +3452,10 @@
         <v>7</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>183</v>
+        <v>225</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>184</v>
+        <v>226</v>
       </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
@@ -3213,13 +3478,13 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>185</v>
+        <v>227</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>126</v>
+        <v>169</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D34" s="1">
         <v>3.5</v>
@@ -3229,10 +3494,10 @@
         <v>7</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>186</v>
+        <v>228</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>187</v>
+        <v>229</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
@@ -3255,13 +3520,13 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>188</v>
+        <v>230</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>130</v>
+        <v>172</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D35" s="1">
         <v>3.5</v>
@@ -3271,10 +3536,10 @@
         <v>7</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>189</v>
+        <v>231</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
@@ -3297,13 +3562,13 @@
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>191</v>
+        <v>233</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>126</v>
+        <v>169</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D36" s="5">
         <v>3.5</v>
@@ -3313,10 +3578,10 @@
         <v>7</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>192</v>
+        <v>234</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>193</v>
+        <v>235</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
@@ -3339,13 +3604,13 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="s">
-        <v>194</v>
+        <v>236</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>70</v>
+        <v>113</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D37" s="5">
         <v>3.5</v>
@@ -3355,10 +3620,10 @@
         <v>7</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>195</v>
+        <v>237</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>196</v>
+        <v>238</v>
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
@@ -3381,13 +3646,13 @@
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>197</v>
+        <v>239</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>198</v>
+        <v>240</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D38" s="5">
         <v>3.5</v>
@@ -3397,10 +3662,10 @@
         <v>7</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>199</v>
+        <v>241</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>200</v>
+        <v>242</v>
       </c>
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
@@ -3423,13 +3688,13 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>201</v>
+        <v>243</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D39" s="5">
         <v>3.5</v>
@@ -3439,10 +3704,10 @@
         <v>7</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>202</v>
+        <v>244</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>203</v>
+        <v>245</v>
       </c>
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
@@ -3465,13 +3730,13 @@
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>204</v>
+        <v>246</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>205</v>
+        <v>247</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>206</v>
+        <v>248</v>
       </c>
       <c r="D40" s="5">
         <v>3.25</v>
@@ -3481,10 +3746,10 @@
         <v>6.5</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>207</v>
+        <v>249</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>208</v>
+        <v>250</v>
       </c>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
@@ -3507,13 +3772,13 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="s">
-        <v>209</v>
+        <v>251</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>210</v>
+        <v>252</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>211</v>
+        <v>253</v>
       </c>
       <c r="D41" s="5">
         <v>3.25</v>
@@ -3523,10 +3788,10 @@
         <v>6.5</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>212</v>
+        <v>254</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>137</v>
+        <v>179</v>
       </c>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
@@ -3549,13 +3814,13 @@
     </row>
     <row r="42">
       <c r="A42" s="5" t="s">
-        <v>213</v>
+        <v>255</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>88</v>
+        <v>131</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="D42" s="5">
         <v>3.25</v>
@@ -3565,10 +3830,10 @@
         <v>6.5</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>214</v>
+        <v>256</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>215</v>
+        <v>257</v>
       </c>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
@@ -3591,13 +3856,13 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="s">
-        <v>216</v>
+        <v>258</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D43" s="5">
         <v>3.25</v>
@@ -3607,10 +3872,10 @@
         <v>6.5</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>217</v>
+        <v>259</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>218</v>
+        <v>260</v>
       </c>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
@@ -3633,13 +3898,13 @@
     </row>
     <row r="44">
       <c r="A44" s="5" t="s">
-        <v>219</v>
+        <v>261</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>135</v>
+        <v>177</v>
       </c>
       <c r="D44" s="5">
         <v>3.25</v>
@@ -3649,10 +3914,10 @@
         <v>6.5</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
@@ -3675,13 +3940,13 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="s">
-        <v>223</v>
+        <v>265</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>130</v>
+        <v>172</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>135</v>
+        <v>177</v>
       </c>
       <c r="D45" s="5">
         <v>3.25</v>
@@ -3691,21 +3956,21 @@
         <v>6.5</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>224</v>
+        <v>266</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>225</v>
+        <v>267</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="5" t="s">
-        <v>226</v>
+        <v>268</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>92</v>
+        <v>135</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D46" s="5">
         <v>3.0</v>
@@ -3715,21 +3980,21 @@
         <v>6</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>227</v>
+        <v>269</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="5" t="s">
-        <v>228</v>
+        <v>270</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>229</v>
+        <v>271</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="D47" s="5">
         <v>3.0</v>
@@ -3739,21 +4004,21 @@
         <v>6</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>230</v>
+        <v>272</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>231</v>
+        <v>273</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="5" t="s">
-        <v>232</v>
+        <v>274</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>233</v>
+        <v>275</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="D48" s="5">
         <v>3.0</v>
@@ -3763,7 +4028,7 @@
         <v>6</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>234</v>
+        <v>276</v>
       </c>
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
@@ -3786,13 +4051,13 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="s">
-        <v>235</v>
+        <v>277</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>163</v>
+        <v>205</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="D49" s="5">
         <v>3.0</v>
@@ -3802,10 +4067,10 @@
         <v>6</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>236</v>
+        <v>278</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>237</v>
+        <v>279</v>
       </c>
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
@@ -3828,13 +4093,13 @@
     </row>
     <row r="50">
       <c r="A50" s="5" t="s">
-        <v>238</v>
+        <v>280</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D50" s="5">
         <v>3.0</v>
@@ -3844,10 +4109,10 @@
         <v>6</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>239</v>
+        <v>281</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>240</v>
+        <v>282</v>
       </c>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
@@ -3870,13 +4135,13 @@
     </row>
     <row r="51">
       <c r="A51" s="5" t="s">
-        <v>241</v>
+        <v>283</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>242</v>
+        <v>284</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="D51" s="5">
         <v>3.0</v>
@@ -3886,10 +4151,10 @@
         <v>6</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>243</v>
+        <v>285</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>242</v>
+        <v>284</v>
       </c>
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
@@ -3912,13 +4177,13 @@
     </row>
     <row r="52">
       <c r="A52" s="5" t="s">
-        <v>244</v>
+        <v>286</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>245</v>
+        <v>287</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>135</v>
+        <v>177</v>
       </c>
       <c r="D52" s="5">
         <v>3.0</v>
@@ -3928,10 +4193,10 @@
         <v>6</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>246</v>
+        <v>288</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>247</v>
+        <v>289</v>
       </c>
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
@@ -3954,13 +4219,13 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="s">
-        <v>248</v>
+        <v>290</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="D53" s="5">
         <v>3.0</v>
@@ -3970,10 +4235,10 @@
         <v>6</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>249</v>
+        <v>291</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>250</v>
+        <v>292</v>
       </c>
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
@@ -3996,13 +4261,13 @@
     </row>
     <row r="54">
       <c r="A54" s="5" t="s">
-        <v>251</v>
+        <v>293</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D54" s="5">
         <v>2.5</v>
@@ -4012,10 +4277,10 @@
         <v>5</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>252</v>
+        <v>294</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>253</v>
+        <v>295</v>
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
@@ -4038,13 +4303,13 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="s">
-        <v>254</v>
+        <v>296</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>163</v>
+        <v>205</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>178</v>
+        <v>220</v>
       </c>
       <c r="D55" s="5">
         <v>2.5</v>
@@ -4054,10 +4319,10 @@
         <v>5</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>255</v>
+        <v>297</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
@@ -4080,13 +4345,13 @@
     </row>
     <row r="56">
       <c r="A56" s="5" t="s">
-        <v>256</v>
+        <v>298</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>257</v>
+        <v>299</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D56" s="5">
         <v>1.5</v>
@@ -4096,10 +4361,10 @@
         <v>3</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>258</v>
+        <v>300</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>259</v>
+        <v>301</v>
       </c>
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
@@ -4122,13 +4387,13 @@
     </row>
     <row r="57">
       <c r="A57" s="5" t="s">
-        <v>260</v>
+        <v>302</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>261</v>
+        <v>303</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D57" s="5">
         <v>0.5</v>
@@ -4138,10 +4403,10 @@
         <v>1</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>262</v>
+        <v>304</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>263</v>
+        <v>305</v>
       </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
@@ -4164,13 +4429,13 @@
     </row>
     <row r="58">
       <c r="A58" s="5" t="s">
-        <v>264</v>
+        <v>306</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>108</v>
+        <v>151</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D58" s="5">
         <v>0.5</v>
@@ -4180,10 +4445,10 @@
         <v>1</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>265</v>
+        <v>307</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>266</v>
+        <v>308</v>
       </c>
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
@@ -4205,7 +4470,7 @@
       <c r="Z58" s="4"/>
     </row>
     <row r="59">
-      <c r="A59" s="4"/>
+      <c r="A59" s="5"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
@@ -29666,22 +29931,22 @@
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>56</v>
+        <v>100</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -29704,13 +29969,13 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>267</v>
+        <v>309</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>268</v>
+        <v>310</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="D2" s="5">
         <v>4.0</v>
@@ -29720,10 +29985,10 @@
         <v>8</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>269</v>
+        <v>311</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>237</v>
+        <v>279</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -29746,13 +30011,13 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>270</v>
+        <v>312</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>271</v>
+        <v>313</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>121</v>
+        <v>164</v>
       </c>
       <c r="D3" s="5">
         <v>4.0</v>
@@ -29762,10 +30027,10 @@
         <v>8</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>272</v>
+        <v>314</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>273</v>
+        <v>315</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -29788,13 +30053,13 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>274</v>
+        <v>316</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>275</v>
+        <v>317</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D4" s="1">
         <v>4.0</v>
@@ -29804,10 +30069,10 @@
         <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>276</v>
+        <v>318</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>277</v>
+        <v>319</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -29830,13 +30095,13 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>278</v>
+        <v>320</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>279</v>
+        <v>321</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="D5" s="1">
         <v>4.0</v>
@@ -29846,21 +30111,21 @@
         <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>280</v>
+        <v>322</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>281</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>282</v>
+        <v>324</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>268</v>
+        <v>310</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>206</v>
+        <v>248</v>
       </c>
       <c r="D6" s="5">
         <v>3.5</v>
@@ -29870,21 +30135,21 @@
         <v>7</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>283</v>
+        <v>325</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>284</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>285</v>
+        <v>327</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>275</v>
+        <v>317</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="D7" s="1">
         <v>3.0</v>
@@ -29894,21 +30159,21 @@
         <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>286</v>
+        <v>328</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>287</v>
+        <v>329</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>288</v>
+        <v>330</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>271</v>
+        <v>313</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D8" s="1">
         <v>3.0</v>
@@ -29918,21 +30183,21 @@
         <v>6</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>289</v>
+        <v>331</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>290</v>
+        <v>332</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>291</v>
+        <v>333</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>275</v>
+        <v>317</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D9" s="1">
         <v>2.5</v>
@@ -29942,21 +30207,21 @@
         <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>292</v>
+        <v>334</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>293</v>
+        <v>335</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>294</v>
+        <v>336</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>178</v>
+        <v>220</v>
       </c>
       <c r="D10" s="1">
         <v>2.0</v>
@@ -29966,21 +30231,21 @@
         <v>4</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>295</v>
+        <v>337</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>296</v>
+        <v>338</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>271</v>
+        <v>313</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D11" s="1">
         <v>2.0</v>
@@ -29990,21 +30255,21 @@
         <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>297</v>
+        <v>339</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>298</v>
+        <v>340</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>271</v>
+        <v>313</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>178</v>
+        <v>220</v>
       </c>
       <c r="D12" s="1">
         <v>3.0</v>
@@ -30014,10 +30279,10 @@
         <v>6</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>299</v>
+        <v>341</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>300</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -30048,22 +30313,22 @@
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>56</v>
+        <v>100</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -30086,13 +30351,13 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>301</v>
+        <v>343</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>302</v>
+        <v>344</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D2" s="1">
         <v>4.5</v>
@@ -30102,21 +30367,21 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>303</v>
+        <v>345</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>304</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>305</v>
+        <v>347</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>306</v>
+        <v>348</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D3" s="1">
         <v>4.0</v>
@@ -30126,21 +30391,21 @@
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>307</v>
+        <v>349</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>308</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>309</v>
+        <v>351</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>306</v>
+        <v>348</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
       <c r="D4" s="1">
         <v>4.0</v>
@@ -30150,21 +30415,21 @@
         <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>310</v>
+        <v>352</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>311</v>
+        <v>353</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>312</v>
+        <v>354</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>313</v>
+        <v>355</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>314</v>
+        <v>356</v>
       </c>
       <c r="D5" s="1">
         <v>4.0</v>
@@ -30174,21 +30439,21 @@
         <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>315</v>
+        <v>357</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>316</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>317</v>
+        <v>358</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>302</v>
+        <v>344</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>314</v>
+        <v>356</v>
       </c>
       <c r="D6" s="1">
         <v>4.0</v>
@@ -30198,15 +30463,15 @@
         <v>8</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>318</v>
+        <v>359</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>319</v>
+        <v>360</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>302</v>
+        <v>344</v>
       </c>
       <c r="D7" s="1">
         <v>4.0</v>
@@ -30216,15 +30481,15 @@
         <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>320</v>
+        <v>361</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>321</v>
+        <v>362</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>302</v>
+        <v>344</v>
       </c>
       <c r="D8" s="1">
         <v>4.0</v>
@@ -30234,18 +30499,18 @@
         <v>8</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>322</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>323</v>
+        <v>364</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>302</v>
+        <v>344</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>314</v>
+        <v>356</v>
       </c>
       <c r="D9" s="1">
         <v>4.0</v>
@@ -30255,18 +30520,18 @@
         <v>8</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>324</v>
+        <v>365</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>325</v>
+        <v>366</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>302</v>
+        <v>344</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>314</v>
+        <v>356</v>
       </c>
       <c r="D10" s="1">
         <v>3.5</v>
@@ -30276,18 +30541,18 @@
         <v>7</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>326</v>
+        <v>367</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>327</v>
+        <v>368</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>306</v>
+        <v>348</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>76</v>
+        <v>119</v>
       </c>
       <c r="D11" s="1">
         <v>3.5</v>
@@ -30297,21 +30562,21 @@
         <v>7</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>328</v>
+        <v>369</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>329</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>330</v>
+        <v>370</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>331</v>
+        <v>371</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>332</v>
+        <v>106</v>
       </c>
       <c r="D12" s="1">
         <v>3.5</v>
@@ -30319,6 +30584,9 @@
       <c r="E12" s="4">
         <f t="shared" si="1"/>
         <v>7</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -30350,21 +30618,21 @@
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>333</v>
+        <v>373</v>
       </c>
       <c r="B2" s="1">
         <v>4.5</v>
@@ -30374,15 +30642,15 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>334</v>
+        <v>374</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>335</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>336</v>
+        <v>376</v>
       </c>
       <c r="B3" s="1">
         <v>4.0</v>
@@ -30392,15 +30660,15 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>337</v>
+        <v>377</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>338</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>339</v>
+        <v>378</v>
       </c>
       <c r="B4" s="1">
         <v>4.0</v>
@@ -30410,15 +30678,15 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>340</v>
+        <v>379</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>341</v>
+        <v>380</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>342</v>
+        <v>381</v>
       </c>
       <c r="B5" s="1">
         <v>4.0</v>
@@ -30428,15 +30696,15 @@
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>343</v>
+        <v>382</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>344</v>
+        <v>383</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>345</v>
+        <v>384</v>
       </c>
       <c r="B6" s="1">
         <v>4.0</v>
@@ -30446,15 +30714,15 @@
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>346</v>
+        <v>385</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>347</v>
+        <v>386</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>348</v>
+        <v>387</v>
       </c>
       <c r="B7" s="1">
         <v>4.0</v>
@@ -30464,15 +30732,15 @@
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>349</v>
+        <v>388</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>350</v>
+        <v>389</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>351</v>
+        <v>390</v>
       </c>
       <c r="B8" s="1">
         <v>4.0</v>
@@ -30482,15 +30750,15 @@
         <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>352</v>
+        <v>391</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>353</v>
+        <v>392</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>354</v>
+        <v>393</v>
       </c>
       <c r="B9" s="1">
         <v>4.0</v>
@@ -30500,15 +30768,15 @@
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>355</v>
+        <v>394</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>356</v>
+        <v>395</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>357</v>
+        <v>396</v>
       </c>
       <c r="B10" s="1">
         <v>3.5</v>
@@ -30518,15 +30786,15 @@
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>358</v>
+        <v>397</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>359</v>
+        <v>398</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>360</v>
+        <v>399</v>
       </c>
       <c r="B11" s="1">
         <v>3.5</v>
@@ -30536,15 +30804,15 @@
         <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>361</v>
+        <v>400</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>362</v>
+        <v>401</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>363</v>
+        <v>402</v>
       </c>
       <c r="B12" s="1">
         <v>3.5</v>
@@ -30554,15 +30822,15 @@
         <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>364</v>
+        <v>403</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>218</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>365</v>
+        <v>404</v>
       </c>
       <c r="B13" s="1">
         <v>3.0</v>
@@ -30572,15 +30840,15 @@
         <v>6</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>366</v>
+        <v>405</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>367</v>
+        <v>406</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>368</v>
+        <v>407</v>
       </c>
       <c r="B14" s="1">
         <v>3.0</v>
@@ -30590,15 +30858,15 @@
         <v>6</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>369</v>
+        <v>408</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>149</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>370</v>
+        <v>409</v>
       </c>
       <c r="B15" s="1">
         <v>2.5</v>
@@ -30608,7 +30876,7 @@
         <v>5</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>371</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>

</xml_diff>